<commit_message>
updated center of mass with new plots
</commit_message>
<xml_diff>
--- a/Density Study/Samara Segment Mass.xlsx
+++ b/Density Study/Samara Segment Mass.xlsx
@@ -3535,7 +3535,9 @@
       <c r="A69" s="4">
         <v>1.0</v>
       </c>
-      <c r="B69" s="4"/>
+      <c r="B69" s="4">
+        <v>352.239669421487</v>
+      </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -3553,12 +3555,17 @@
       <c r="A70" s="4">
         <v>2.0</v>
       </c>
+      <c r="B70" s="4">
+        <v>504.270531400966</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="4">
         <v>3.0</v>
       </c>
-      <c r="B71" s="4"/>
+      <c r="B71" s="4">
+        <v>565.137346938775</v>
+      </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -3581,73 +3588,112 @@
       <c r="A72" s="4">
         <v>4.0</v>
       </c>
+      <c r="B72" s="4">
+        <v>332.905671296296</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="4">
         <v>5.0</v>
       </c>
+      <c r="B73" s="4">
+        <v>649.214078859434</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="4">
         <v>6.0</v>
       </c>
+      <c r="B74" s="4">
+        <v>615.777233236801</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="4">
         <v>7.0</v>
       </c>
+      <c r="B75" s="4">
+        <v>532.90478079746</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="4">
         <v>8.0</v>
       </c>
+      <c r="B76" s="4">
+        <v>388.81663516068</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="4">
         <v>9.0</v>
       </c>
+      <c r="B77" s="4">
+        <v>567.150590331922</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="4">
         <v>10.0</v>
       </c>
+      <c r="B78" s="4">
+        <v>545.177346938775</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="4">
         <v>11.0</v>
       </c>
+      <c r="B79" s="4">
+        <v>421.778197857592</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="4">
         <v>12.0</v>
       </c>
+      <c r="B80" s="4">
+        <v>442.411672978391</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="4">
         <v>13.0</v>
       </c>
+      <c r="B81" s="4">
+        <v>502.466326530612</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="4">
         <v>14.0</v>
       </c>
+      <c r="B82" s="4">
+        <v>628.646944444444</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="4">
         <v>15.0</v>
       </c>
+      <c r="B83" s="4">
+        <v>565.516219723183</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="4">
         <v>16.0</v>
       </c>
+      <c r="B84" s="4">
+        <v>396.082647462277</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="4">
         <v>17.0</v>
       </c>
       <c r="B85" s="4">
-        <v>611.590449954086</v>
+        <v>477.320501730103</v>
       </c>
     </row>
     <row r="86">
@@ -3655,7 +3701,7 @@
         <v>18.0</v>
       </c>
       <c r="B86" s="4">
-        <v>710.88062283737</v>
+        <v>566.722130177514</v>
       </c>
     </row>
     <row r="87">
@@ -3663,7 +3709,7 @@
         <v>19.0</v>
       </c>
       <c r="B87" s="4">
-        <v>164.931836734693</v>
+        <v>257.26275510204</v>
       </c>
     </row>
     <row r="88">
@@ -3671,7 +3717,7 @@
         <v>20.0</v>
       </c>
       <c r="B88" s="4">
-        <v>711.866326530612</v>
+        <v>510.385637770283</v>
       </c>
     </row>
     <row r="89">
@@ -3679,7 +3725,7 @@
         <v>21.0</v>
       </c>
       <c r="B89" s="4">
-        <v>703.287839714342</v>
+        <v>570.082040816326</v>
       </c>
     </row>
     <row r="90">
@@ -3687,7 +3733,7 @@
         <v>22.0</v>
       </c>
       <c r="B90" s="4">
-        <v>883.020049008687</v>
+        <v>616.135290616941</v>
       </c>
     </row>
     <row r="91">
@@ -3695,7 +3741,7 @@
         <v>23.0</v>
       </c>
       <c r="B91" s="4">
-        <v>343.442344045368</v>
+        <v>320.80574845679</v>
       </c>
     </row>
     <row r="92">
@@ -3703,7 +3749,7 @@
         <v>24.0</v>
       </c>
       <c r="B92" s="4">
-        <v>708.620408163265</v>
+        <v>522.467959183673</v>
       </c>
     </row>
     <row r="93">
@@ -3711,7 +3757,7 @@
         <v>25.0</v>
       </c>
       <c r="B93" s="4">
-        <v>652.136480856972</v>
+        <v>486.636734693877</v>
       </c>
     </row>
     <row r="94">
@@ -3719,7 +3765,7 @@
         <v>26.0</v>
       </c>
       <c r="B94" s="4">
-        <v>766.225346020761</v>
+        <v>557.247551020408</v>
       </c>
     </row>
     <row r="95">

</xml_diff>

<commit_message>
Updated spreadsheet and code to add 3D printed samaras
</commit_message>
<xml_diff>
--- a/Density Study/Samara Segment Mass.xlsx
+++ b/Density Study/Samara Segment Mass.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Segment mass (mg) Seed to Wing</t>
   </si>
@@ -26,6 +26,33 @@
   </si>
   <si>
     <t>Area mm^2 (TOTAL)</t>
+  </si>
+  <si>
+    <t>Wing Loading (N/m^2)</t>
+  </si>
+  <si>
+    <t>3D Printed PLA</t>
+  </si>
+  <si>
+    <t>Mass mg</t>
+  </si>
+  <si>
+    <t>Total Mass</t>
+  </si>
+  <si>
+    <t>1 (24)</t>
+  </si>
+  <si>
+    <t>2 (12)</t>
+  </si>
+  <si>
+    <t>Length mm</t>
+  </si>
+  <si>
+    <t>Total Area mm^2</t>
+  </si>
+  <si>
+    <t>Wing Loading N/m^2</t>
   </si>
 </sst>
 </file>
@@ -90,6 +117,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -3530,6 +3558,9 @@
       <c r="B68" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E68" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="4">
@@ -3540,7 +3571,10 @@
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
+      <c r="E69" s="4">
+        <f t="shared" ref="E69:E98" si="2">W5*10^-6*9.81/(B69*10^-6)</f>
+        <v>1.32567692</v>
+      </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
@@ -3558,6 +3592,10 @@
       <c r="B70" s="4">
         <v>504.270531400966</v>
       </c>
+      <c r="E70" s="4">
+        <f t="shared" si="2"/>
+        <v>2.069888948</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="4">
@@ -3568,7 +3606,10 @@
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
+      <c r="E71" s="4">
+        <f t="shared" si="2"/>
+        <v>2.218430629</v>
+      </c>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
@@ -3591,6 +3632,10 @@
       <c r="B72" s="4">
         <v>332.905671296296</v>
       </c>
+      <c r="E72" s="4">
+        <f t="shared" si="2"/>
+        <v>1.293636718</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="4">
@@ -3599,6 +3644,10 @@
       <c r="B73" s="4">
         <v>649.214078859434</v>
       </c>
+      <c r="E73" s="4">
+        <f t="shared" si="2"/>
+        <v>2.030861688</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="4">
@@ -3607,6 +3656,10 @@
       <c r="B74" s="4">
         <v>615.777233236801</v>
       </c>
+      <c r="E74" s="4">
+        <f t="shared" si="2"/>
+        <v>2.066261842</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="4">
@@ -3615,6 +3668,10 @@
       <c r="B75" s="4">
         <v>532.90478079746</v>
       </c>
+      <c r="E75" s="4">
+        <f t="shared" si="2"/>
+        <v>2.185093927</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="4">
@@ -3623,6 +3680,10 @@
       <c r="B76" s="4">
         <v>388.81663516068</v>
       </c>
+      <c r="E76" s="4">
+        <f t="shared" si="2"/>
+        <v>3.234537533</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="4">
@@ -3631,6 +3692,10 @@
       <c r="B77" s="4">
         <v>567.150590331922</v>
       </c>
+      <c r="E77" s="4">
+        <f t="shared" si="2"/>
+        <v>1.807535807</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="4">
@@ -3639,6 +3704,10 @@
       <c r="B78" s="4">
         <v>545.177346938775</v>
       </c>
+      <c r="E78" s="4">
+        <f t="shared" si="2"/>
+        <v>2.294253433</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="4">
@@ -3647,6 +3716,10 @@
       <c r="B79" s="4">
         <v>421.778197857592</v>
       </c>
+      <c r="E79" s="4">
+        <f t="shared" si="2"/>
+        <v>1.279226861</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="4">
@@ -3655,6 +3728,10 @@
       <c r="B80" s="4">
         <v>442.411672978391</v>
       </c>
+      <c r="E80" s="4">
+        <f t="shared" si="2"/>
+        <v>2.643130983</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="4">
@@ -3663,6 +3740,10 @@
       <c r="B81" s="4">
         <v>502.466326530612</v>
       </c>
+      <c r="E81" s="4">
+        <f t="shared" si="2"/>
+        <v>2.565413704</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="4">
@@ -3671,6 +3752,10 @@
       <c r="B82" s="4">
         <v>628.646944444444</v>
       </c>
+      <c r="E82" s="4">
+        <f t="shared" si="2"/>
+        <v>2.49054897</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="4">
@@ -3679,6 +3764,10 @@
       <c r="B83" s="4">
         <v>565.516219723183</v>
       </c>
+      <c r="E83" s="4">
+        <f t="shared" si="2"/>
+        <v>1.817963772</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="4">
@@ -3687,6 +3776,10 @@
       <c r="B84" s="4">
         <v>396.082647462277</v>
       </c>
+      <c r="E84" s="4">
+        <f t="shared" si="2"/>
+        <v>1.270575733</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="4">
@@ -3695,6 +3788,10 @@
       <c r="B85" s="4">
         <v>477.320501730103</v>
       </c>
+      <c r="E85" s="4">
+        <f t="shared" si="2"/>
+        <v>2.155928765</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="4">
@@ -3703,6 +3800,10 @@
       <c r="B86" s="4">
         <v>566.722130177514</v>
       </c>
+      <c r="E86" s="4">
+        <f t="shared" si="2"/>
+        <v>1.746586109</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="4">
@@ -3711,6 +3812,10 @@
       <c r="B87" s="4">
         <v>257.26275510204</v>
       </c>
+      <c r="E87" s="4">
+        <f t="shared" si="2"/>
+        <v>2.40995631</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="4">
@@ -3719,6 +3824,10 @@
       <c r="B88" s="4">
         <v>510.385637770283</v>
       </c>
+      <c r="E88" s="4">
+        <f t="shared" si="2"/>
+        <v>2.293036703</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="4">
@@ -3727,6 +3836,10 @@
       <c r="B89" s="4">
         <v>570.082040816326</v>
       </c>
+      <c r="E89" s="4">
+        <f t="shared" si="2"/>
+        <v>1.731129784</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="4">
@@ -3735,6 +3848,10 @@
       <c r="B90" s="4">
         <v>616.135290616941</v>
       </c>
+      <c r="E90" s="4">
+        <f t="shared" si="2"/>
+        <v>2.190843506</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="4">
@@ -3743,6 +3860,10 @@
       <c r="B91" s="4">
         <v>320.80574845679</v>
       </c>
+      <c r="E91" s="4">
+        <f t="shared" si="2"/>
+        <v>2.629815719</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="4">
@@ -3751,6 +3872,10 @@
       <c r="B92" s="4">
         <v>522.467959183673</v>
       </c>
+      <c r="E92" s="4">
+        <f t="shared" si="2"/>
+        <v>2.521653198</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="4">
@@ -3759,6 +3884,10 @@
       <c r="B93" s="4">
         <v>486.636734693877</v>
       </c>
+      <c r="E93" s="4">
+        <f t="shared" si="2"/>
+        <v>2.106591893</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="4">
@@ -3767,6 +3896,10 @@
       <c r="B94" s="4">
         <v>557.247551020408</v>
       </c>
+      <c r="E94" s="4">
+        <f t="shared" si="2"/>
+        <v>1.994576733</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="4">
@@ -3775,6 +3908,10 @@
       <c r="B95" s="4">
         <v>427.082324935528</v>
       </c>
+      <c r="E95" s="4">
+        <f t="shared" si="2"/>
+        <v>1.258745606</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="4">
@@ -3783,6 +3920,10 @@
       <c r="B96" s="4">
         <v>517.936326530612</v>
       </c>
+      <c r="E96" s="4">
+        <f t="shared" si="2"/>
+        <v>1.738742687</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="4">
@@ -3791,6 +3932,10 @@
       <c r="B97" s="4">
         <v>273.359429065743</v>
       </c>
+      <c r="E97" s="4">
+        <f t="shared" si="2"/>
+        <v>2.580262193</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="4">
@@ -3798,6 +3943,388 @@
       </c>
       <c r="B98" s="4">
         <v>337.266734693877</v>
+      </c>
+      <c r="E98" s="4">
+        <f t="shared" si="2"/>
+        <v>2.833051415</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="D99" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C100" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D100" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E100" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F100" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G100" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="H100" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I100" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J100" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="K100" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="L100" s="4">
+        <v>11.0</v>
+      </c>
+      <c r="M100" s="4">
+        <v>12.0</v>
+      </c>
+      <c r="N100" s="4">
+        <v>13.0</v>
+      </c>
+      <c r="O100" s="4">
+        <v>14.0</v>
+      </c>
+      <c r="P100" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="Q100" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="R100" s="4">
+        <v>17.0</v>
+      </c>
+      <c r="S100" s="4">
+        <v>18.0</v>
+      </c>
+      <c r="T100" s="4">
+        <v>19.0</v>
+      </c>
+      <c r="U100" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="W100" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B101" s="4">
+        <v>22.6</v>
+      </c>
+      <c r="C101" s="4">
+        <v>21.5</v>
+      </c>
+      <c r="D101" s="4">
+        <v>31.0</v>
+      </c>
+      <c r="E101" s="4">
+        <v>33.9</v>
+      </c>
+      <c r="F101" s="4">
+        <v>16.9</v>
+      </c>
+      <c r="G101" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="H101" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="I101" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="J101" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="K101" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="L101" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="M101" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="N101" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="O101" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="P101" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="Q101" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="R101" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="S101" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="T101" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="U101" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="W101">
+        <f t="shared" ref="W101:W102" si="3">SUM(B101:U101)</f>
+        <v>185.2</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B102" s="4">
+        <v>27.0</v>
+      </c>
+      <c r="C102" s="4">
+        <v>28.3</v>
+      </c>
+      <c r="D102" s="4">
+        <v>30.6</v>
+      </c>
+      <c r="E102" s="4">
+        <v>24.7</v>
+      </c>
+      <c r="F102" s="4">
+        <v>14.2</v>
+      </c>
+      <c r="G102" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="H102" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="I102" s="4">
+        <v>5.1</v>
+      </c>
+      <c r="J102" s="4">
+        <v>5.8</v>
+      </c>
+      <c r="K102" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="L102" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="M102" s="4">
+        <v>4.9</v>
+      </c>
+      <c r="N102" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="O102" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="P102" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="Q102" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="R102" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="S102" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="T102" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="U102" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="W102">
+        <f t="shared" si="3"/>
+        <v>181.9</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="B104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="H104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="I104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="J104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="K104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="M104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="N104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="O104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="P104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="Q104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="R104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="S104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="T104" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="U104" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="B105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="F105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="H105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="I105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="J105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="K105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="M105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="N105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="O105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="P105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="Q105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="R105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="S105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="T105" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="U105" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="B107" s="4">
+        <v>554.577780214358</v>
+      </c>
+      <c r="E107">
+        <f t="shared" ref="E107:E108" si="4">W101*10^-6*9.81/(B107*10^-6)</f>
+        <v>3.276027394</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="B108" s="4">
+        <v>577.386823006657</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="4"/>
+        <v>3.090543339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>